<commit_message>
Generating and pushing into server. Also deploys functions
</commit_message>
<xml_diff>
--- a/Generators/json.xlsx
+++ b/Generators/json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\suresh\git\Uyamak\Generators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6109255F-0CCE-4DEB-95B5-084AEF823E3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F797FF35-F6A2-46B4-9862-CD8ABE1F87B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB8984A2-0721-4967-8668-669096886DF4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>newFile</t>
   </si>
@@ -141,13 +141,16 @@
     <t>display</t>
   </si>
   <si>
-    <t>top</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
-    <t>ture</t>
+    <t>order</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -500,15 +503,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368AF13B-AD09-4EC1-B187-55BF9EDB6D77}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -525,17 +528,20 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="str">
-        <f ca="1">CHAR(34)&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;CHAR(34)&amp;":{"&amp;_xlfn.CONCAT(H:H)&amp;"}"</f>
-        <v>"tools":{"newFile":{"icon":"fas fa-file","function":"openLeftMenu()","text":"New file","display":"ture","top":"0","left":"0"},"saveFile":{"icon":"far fa-save","function":"openLeftMenu()","text":"Save file","display":"ture","top":"0","left":"40"},"deleteFile":{"icon":"far fa-trash-alt","function":"openLeftMenu()","text":"Delete file","display":"ture","top":"0","left":"80"},"addBlock":{"icon":"far fa-plus-square","function":"openLeftMenu()","text":"Add block","display":"ture","top":"0","left":"120"},"editBlock":{"icon":"far fa-edit","function":"openLeftMenu()","text":"Edit block","display":"ture","top":"0","left":"160"},"addConnection":{"icon":"fas fa-project-diagram","function":"openLeftMenu()","text":"Add connection","display":"ture","top":"0","left":"200"},"editConnection":{"icon":"fas fa-pencil-alt","function":"openLeftMenu()","text":"Edit connection","display":"ture","top":"0","left":"240"},"delete":{"icon":"fas fa-eraser","function":"openLeftMenu()","text":"Delete","display":"ture","top":"0","left":"280"},"filesView":{"icon":"far fa-folder-open","function":"openLeftMenu()","text":"Files view","display":"ture","top":"0","left":"320"},"simView":{"icon":"fas fa-play","function":"openLeftMenu()","text":"Simulation view","display":"ture","top":"0","left":"360"}}</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="str">
+        <f ca="1">CHAR(34)&amp;MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)&amp;CHAR(34)&amp;":{"&amp;_xlfn.CONCAT(I:I)&amp;"}"</f>
+        <v>"tools":{"newFile":{"icon":"fas fa-file","function":"openLeftMenu()","text":"New file","display":"false","y":"0","x":"0","order":"0"},"saveFile":{"icon":"far fa-save","function":"openLeftMenu()","text":"Save file","display":"false","y":"0","x":"40","order":"1"},"deleteFile":{"icon":"far fa-trash-alt","function":"openLeftMenu()","text":"Delete file","display":"false","y":"0","x":"80","order":"2"},"addBlock":{"icon":"far fa-plus-square","function":"openLeftMenu()","text":"Add block","display":"false","y":"0","x":"120","order":"3"},"editBlock":{"icon":"far fa-edit","function":"openLeftMenu()","text":"Edit block","display":"false","y":"0","x":"160","order":"4"},"addConnection":{"icon":"fas fa-project-diagram","function":"openLeftMenu()","text":"Add connection","display":"false","y":"0","x":"200","order":"5"},"editConnection":{"icon":"fas fa-pencil-alt","function":"openLeftMenu()","text":"Edit connection","display":"false","y":"0","x":"240","order":"6"},"delete":{"icon":"fas fa-eraser","function":"openLeftMenu()","text":"Delete","display":"false","y":"0","x":"280","order":"7"},"filesView":{"icon":"far fa-folder-open","function":"openLeftMenu()","text":"Files view","display":"false","y":"0","x":"320","order":"8"},"simView":{"icon":"fas fa-play","function":"openLeftMenu()","text":"Simulation view","display":"false","y":"0","x":"360","order":"9"}}</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -549,7 +555,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -557,12 +563,15 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="str">
-        <f>CHAR(34)&amp;A2&amp;CHAR(34)&amp;":{"&amp;CHAR(34)&amp;$B$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$C$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$D$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$E$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$F$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;F2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$G$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;G2&amp;CHAR(34)&amp;"}"&amp;IF(ISBLANK(A3),"",",")</f>
-        <v>"newFile":{"icon":"fas fa-file","function":"openLeftMenu()","text":"New file","display":"ture","top":"0","left":"0"},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CHAR(34)&amp;A2&amp;CHAR(34)&amp;":{"&amp;CHAR(34)&amp;$B$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$C$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$D$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;D2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$E$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;E2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$F$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;F2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$G$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;G2&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$H$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;H2&amp;CHAR(34)&amp;"}"&amp;IF(ISBLANK(A3),"",",")</f>
+        <v>"newFile":{"icon":"fas fa-file","function":"openLeftMenu()","text":"New file","display":"false","y":"0","x":"0","order":"0"},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -575,8 +584,9 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>38</v>
+      <c r="E3" s="1" t="str">
+        <f>E2</f>
+        <v>false</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -585,12 +595,15 @@
         <f>+G2+40</f>
         <v>40</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H11" si="0">CHAR(34)&amp;A3&amp;CHAR(34)&amp;":{"&amp;CHAR(34)&amp;$B$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$C$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$D$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$E$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;E3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$F$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;F3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$G$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;G3&amp;CHAR(34)&amp;"}"&amp;IF(ISBLANK(A4),"",",")</f>
-        <v>"saveFile":{"icon":"far fa-save","function":"openLeftMenu()","text":"Save file","display":"ture","top":"0","left":"40"},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I11" si="0">CHAR(34)&amp;A3&amp;CHAR(34)&amp;":{"&amp;CHAR(34)&amp;$B$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$C$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$D$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;D3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$E$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;E3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$F$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;F3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$G$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;G3&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;$H$1&amp;CHAR(34)&amp;":"&amp;CHAR(34)&amp;H3&amp;CHAR(34)&amp;"}"&amp;IF(ISBLANK(A4),"",",")</f>
+        <v>"saveFile":{"icon":"far fa-save","function":"openLeftMenu()","text":"Save file","display":"false","y":"0","x":"40","order":"1"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -603,22 +616,26 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4:E11" si="1">E3</f>
+        <v>false</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G11" si="1">+G3+40</f>
+        <f t="shared" ref="G4:G11" si="2">+G3+40</f>
         <v>80</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>"deleteFile":{"icon":"far fa-trash-alt","function":"openLeftMenu()","text":"Delete file","display":"ture","top":"0","left":"80"},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"deleteFile":{"icon":"far fa-trash-alt","function":"openLeftMenu()","text":"Delete file","display":"false","y":"0","x":"80","order":"2"},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -631,22 +648,26 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>"addBlock":{"icon":"far fa-plus-square","function":"openLeftMenu()","text":"Add block","display":"ture","top":"0","left":"120"},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"addBlock":{"icon":"far fa-plus-square","function":"openLeftMenu()","text":"Add block","display":"false","y":"0","x":"120","order":"3"},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -659,22 +680,26 @@
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>"editBlock":{"icon":"far fa-edit","function":"openLeftMenu()","text":"Edit block","display":"ture","top":"0","left":"160"},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"editBlock":{"icon":"far fa-edit","function":"openLeftMenu()","text":"Edit block","display":"false","y":"0","x":"160","order":"4"},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -687,22 +712,26 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>"addConnection":{"icon":"fas fa-project-diagram","function":"openLeftMenu()","text":"Add connection","display":"ture","top":"0","left":"200"},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"addConnection":{"icon":"fas fa-project-diagram","function":"openLeftMenu()","text":"Add connection","display":"false","y":"0","x":"200","order":"5"},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -715,22 +744,26 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>38</v>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="H8" t="str">
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>"editConnection":{"icon":"fas fa-pencil-alt","function":"openLeftMenu()","text":"Edit connection","display":"ture","top":"0","left":"240"},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"editConnection":{"icon":"fas fa-pencil-alt","function":"openLeftMenu()","text":"Edit connection","display":"false","y":"0","x":"240","order":"6"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -743,22 +776,26 @@
       <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>280</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>"delete":{"icon":"fas fa-eraser","function":"openLeftMenu()","text":"Delete","display":"ture","top":"0","left":"280"},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"delete":{"icon":"fas fa-eraser","function":"openLeftMenu()","text":"Delete","display":"false","y":"0","x":"280","order":"7"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -771,22 +808,26 @@
       <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>38</v>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>320</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>"filesView":{"icon":"far fa-folder-open","function":"openLeftMenu()","text":"Files view","display":"ture","top":"0","left":"320"},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>"filesView":{"icon":"far fa-folder-open","function":"openLeftMenu()","text":"Files view","display":"false","y":"0","x":"320","order":"8"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -799,19 +840,23 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>"simView":{"icon":"fas fa-play","function":"openLeftMenu()","text":"Simulation view","display":"ture","top":"0","left":"360"}</v>
+        <v>"simView":{"icon":"fas fa-play","function":"openLeftMenu()","text":"Simulation view","display":"false","y":"0","x":"360","order":"9"}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>